<commit_message>
added tta mechanism + ensemble of res34+101
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76358E05-1E99-43AE-BB5D-19B6AC53350D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6FC922-1465-4347-8B48-BF775BD9584D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,16 +25,16 @@
     <t>Finetune the third fold of the best model (CV5_resnet34_mixed_loss_no_drop model-2.pt?=</t>
   </si>
   <si>
-    <t>Add TTA to predictions</t>
-  </si>
-  <si>
     <t>Add classifier of empty predictions</t>
   </si>
   <si>
-    <t>Ensemble with resnet101</t>
-  </si>
-  <si>
     <t>Remove few pixel images and retrain</t>
+  </si>
+  <si>
+    <t>Ensemble with resnet101 OK</t>
+  </si>
+  <si>
+    <t>Add TTA to predictions OK</t>
   </si>
 </sst>
 </file>
@@ -355,7 +355,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -367,12 +367,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -382,7 +382,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>